<commit_message>
update illustrative MODS for Banks image
</commit_message>
<xml_diff>
--- a/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative-MODS-04.0.xlsx
+++ b/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative-MODS-04.0.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24500" windowHeight="15380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13190" uniqueCount="3282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13199" uniqueCount="3287">
   <si>
     <t>liv_013001</t>
   </si>
@@ -9865,6 +9865,21 @@
   </si>
   <si>
     <t>Adrian S. Wisnicki, Justin Livingstone, and Heather F. Ball at University of Glasgow Library, 2017</t>
+  </si>
+  <si>
+    <t>liv_016252</t>
+  </si>
+  <si>
+    <t>Nigel Banks</t>
+  </si>
+  <si>
+    <t>Nigel Banks, 2017</t>
+  </si>
+  <si>
+    <t>Banks, Nigel</t>
+  </si>
+  <si>
+    <t>&amp;#169; Nigel Banks. Creative Commons Attribution-NonCommercial 3.0 Unported (https://creativecommons.org/licenses/by-nc/3.0/).</t>
   </si>
 </sst>
 </file>
@@ -9877,6 +9892,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10011,7 +10027,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="838">
+  <cellStyleXfs count="844">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -10073,6 +10089,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11064,7 +11086,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="838">
+  <cellStyles count="844">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -11492,6 +11514,9 @@
     <cellStyle name="Followed Hyperlink" xfId="833" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="835" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="837" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="839" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="841" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="843" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -11902,6 +11927,9 @@
     <cellStyle name="Hyperlink" xfId="832" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="834" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="836" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="838" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="840" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="842" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -12231,11 +12259,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1191"/>
+  <dimension ref="A1:P1192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1170" sqref="C1170:C1191"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1187" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1192" sqref="A1192:P1192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -60743,6 +60771,41 @@
         <v>2579</v>
       </c>
     </row>
+    <row r="1192" spans="1:16" ht="45">
+      <c r="A1192" s="28" t="s">
+        <v>3282</v>
+      </c>
+      <c r="B1192" s="22" t="s">
+        <v>3283</v>
+      </c>
+      <c r="C1192" s="9" t="s">
+        <v>3284</v>
+      </c>
+      <c r="F1192" s="9" t="s">
+        <v>3285</v>
+      </c>
+      <c r="G1192" s="9" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1192" s="69" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1192" s="69" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1192" s="70">
+        <v>2017</v>
+      </c>
+      <c r="K1192" s="70">
+        <v>2017</v>
+      </c>
+      <c r="L1192" s="70" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P1192" s="69" t="s">
+        <v>3286</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
illus 16259 MODS + DC
</commit_message>
<xml_diff>
--- a/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative-MODS-04.0.xlsx
+++ b/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative-MODS-04.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24960" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24940" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13253" uniqueCount="3305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13262" uniqueCount="3310">
   <si>
     <t>liv_013001</t>
   </si>
@@ -9934,6 +9934,21 @@
   </si>
   <si>
     <t>&amp;#169; Neil R. Lindsay. Courtesy of Neil R. Lindsay.</t>
+  </si>
+  <si>
+    <t>liv_016259</t>
+  </si>
+  <si>
+    <t>Heather F. Ball, 2017</t>
+  </si>
+  <si>
+    <t>Heather F. Ball</t>
+  </si>
+  <si>
+    <t>Rodriguez, Andreina</t>
+  </si>
+  <si>
+    <t>&amp;#169; The Torch/Andreina Rodriguez. Courtesy of St. John's University.</t>
   </si>
 </sst>
 </file>
@@ -10081,7 +10096,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="874">
+  <cellStyleXfs count="876">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -10143,6 +10158,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11170,7 +11187,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="874">
+  <cellStyles count="876">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -11616,6 +11633,7 @@
     <cellStyle name="Followed Hyperlink" xfId="869" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="871" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="873" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="875" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -12044,6 +12062,7 @@
     <cellStyle name="Hyperlink" xfId="868" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="870" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="872" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="874" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -12375,9 +12394,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1190" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1198" sqref="C1193:C1198"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1195" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1200" sqref="P1200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -61130,8 +61149,40 @@
         <v>3304</v>
       </c>
     </row>
-    <row r="1199" spans="1:16">
-      <c r="A1199" s="28"/>
+    <row r="1199" spans="1:16" ht="45">
+      <c r="A1199" s="28" t="s">
+        <v>3305</v>
+      </c>
+      <c r="B1199" s="22" t="s">
+        <v>3307</v>
+      </c>
+      <c r="C1199" s="9" t="s">
+        <v>3306</v>
+      </c>
+      <c r="F1199" s="9" t="s">
+        <v>3308</v>
+      </c>
+      <c r="G1199" s="9" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1199" s="69" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1199" s="69" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1199" s="70">
+        <v>2017</v>
+      </c>
+      <c r="K1199" s="70">
+        <v>2017</v>
+      </c>
+      <c r="L1199" s="70" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P1199" s="9" t="s">
+        <v>3309</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
illus MODCS+ DC xlsx
</commit_message>
<xml_diff>
--- a/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative-MODS-04.0.xlsx
+++ b/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative-MODS-04.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24940" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24680" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13262" uniqueCount="3310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13280" uniqueCount="3318">
   <si>
     <t>liv_013001</t>
   </si>
@@ -9949,6 +9949,30 @@
   </si>
   <si>
     <t>&amp;#169; The Torch/Andreina Rodriguez. Courtesy of St. John's University.</t>
+  </si>
+  <si>
+    <t>liv_016260</t>
+  </si>
+  <si>
+    <t>liv_016261</t>
+  </si>
+  <si>
+    <t>Silicified trees: Dadoxylon (left and center) and Rhexoxylon (right) from area due south of Zumbo, South Africa, 2018</t>
+  </si>
+  <si>
+    <t>Silicified trees: Dadoxylon (left and center) and Rhexoxylon (right) from area due south of Zumbo, South Africa</t>
+  </si>
+  <si>
+    <t>Memorial in the old Simonstown Naval Cemetery, South Africa</t>
+  </si>
+  <si>
+    <t>Memorial in the old Simonstown Naval Cemetery, South Africa, 2018</t>
+  </si>
+  <si>
+    <t>Walter, Lewis</t>
+  </si>
+  <si>
+    <t>&amp;#169; Lewis Walter. Used by permission.</t>
   </si>
 </sst>
 </file>
@@ -9961,7 +9985,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10096,7 +10119,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="876">
+  <cellStyleXfs count="898">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -10158,6 +10181,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11187,7 +11232,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="876">
+  <cellStyles count="898">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -11634,6 +11679,17 @@
     <cellStyle name="Followed Hyperlink" xfId="871" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="873" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="875" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="877" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="879" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="881" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="883" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="885" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="887" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="889" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="891" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="893" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="895" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="897" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -12063,6 +12119,17 @@
     <cellStyle name="Hyperlink" xfId="870" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="872" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="874" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="876" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="878" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="880" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="882" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="884" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="886" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="888" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="890" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="892" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="894" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="896" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -12392,11 +12459,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1199"/>
+  <dimension ref="A1:P1201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1195" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1200" sqref="P1200"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1201" sqref="P1201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -61184,6 +61251,76 @@
         <v>3309</v>
       </c>
     </row>
+    <row r="1200" spans="1:16" ht="45">
+      <c r="A1200" s="28" t="s">
+        <v>3310</v>
+      </c>
+      <c r="B1200" s="22" t="s">
+        <v>3314</v>
+      </c>
+      <c r="C1200" s="22" t="s">
+        <v>3315</v>
+      </c>
+      <c r="F1200" s="9" t="s">
+        <v>3316</v>
+      </c>
+      <c r="G1200" s="9" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1200" s="69" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1200" s="69" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1200" s="70">
+        <v>2018</v>
+      </c>
+      <c r="K1200" s="70">
+        <v>2018</v>
+      </c>
+      <c r="L1200" s="70" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P1200" s="9" t="s">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:16" ht="45">
+      <c r="A1201" s="28" t="s">
+        <v>3311</v>
+      </c>
+      <c r="B1201" s="22" t="s">
+        <v>3313</v>
+      </c>
+      <c r="C1201" s="22" t="s">
+        <v>3312</v>
+      </c>
+      <c r="F1201" s="9" t="s">
+        <v>3316</v>
+      </c>
+      <c r="G1201" s="9" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1201" s="69" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1201" s="69" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1201" s="70">
+        <v>2018</v>
+      </c>
+      <c r="K1201" s="70">
+        <v>2018</v>
+      </c>
+      <c r="L1201" s="70" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P1201" s="9" t="s">
+        <v>3317</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add slave stick Illus MODS
</commit_message>
<xml_diff>
--- a/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative-MODS-04.0.xlsx
+++ b/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative-MODS-04.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24680" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13280" uniqueCount="3318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13294" uniqueCount="3322">
   <si>
     <t>liv_013001</t>
   </si>
@@ -9973,6 +9973,18 @@
   </si>
   <si>
     <t>&amp;#169; Lewis Walter. Used by permission.</t>
+  </si>
+  <si>
+    <t>liv_016262</t>
+  </si>
+  <si>
+    <t>Slave stick, reportedly removed by David Livingstone from the neck of a slave</t>
+  </si>
+  <si>
+    <t>Slave stick, reportedly removed by David Livingstone from the neck of a slave, 1840-1870</t>
+  </si>
+  <si>
+    <t>&amp;#169; David Livingstone Centre. May not be reproduced without the express written consent of the National Trust for Scotland, on behalf of the Scottish National Memorial to David Livingstone Trust.</t>
   </si>
 </sst>
 </file>
@@ -10119,7 +10131,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="898">
+  <cellStyleXfs count="916">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -10181,6 +10193,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11232,7 +11262,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="898">
+  <cellStyles count="916">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -11690,6 +11720,15 @@
     <cellStyle name="Followed Hyperlink" xfId="893" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="895" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="897" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="899" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="901" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="903" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="905" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="907" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="909" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="911" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="913" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="915" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -12130,6 +12169,15 @@
     <cellStyle name="Hyperlink" xfId="892" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="894" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="896" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="898" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="900" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="902" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="904" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="906" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="908" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="910" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="912" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="914" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -12459,11 +12507,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1201"/>
+  <dimension ref="A1:P1202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1194" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1201" sqref="P1201"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1198" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1202" sqref="P1202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -61321,6 +61369,52 @@
         <v>3317</v>
       </c>
     </row>
+    <row r="1202" spans="1:16" ht="60">
+      <c r="A1202" s="28" t="s">
+        <v>3318</v>
+      </c>
+      <c r="B1202" s="22" t="s">
+        <v>3319</v>
+      </c>
+      <c r="C1202" s="22" t="s">
+        <v>3320</v>
+      </c>
+      <c r="D1202" s="11" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E1202" s="5"/>
+      <c r="F1202" s="5"/>
+      <c r="G1202" s="5" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1202" s="5" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1202" s="5" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1202" s="4" t="s">
+        <v>1203</v>
+      </c>
+      <c r="K1202" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="L1202" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="M1202" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1202" s="7" t="s">
+        <v>1150</v>
+      </c>
+      <c r="O1202" s="6" t="s">
+        <v>1148</v>
+      </c>
+      <c r="P1202" s="5" t="s">
+        <v>3321</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
update Illustrative MODS excel
</commit_message>
<xml_diff>
--- a/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative-MODS-04.0.xlsx
+++ b/MODS-DC-Generators/Illustrative-MODS-Generator-NEW/Illustrative-MODS-04.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24660" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13294" uniqueCount="3322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13359" uniqueCount="3337">
   <si>
     <t>liv_013001</t>
   </si>
@@ -9985,6 +9985,51 @@
   </si>
   <si>
     <t>&amp;#169; David Livingstone Centre. May not be reproduced without the express written consent of the National Trust for Scotland, on behalf of the Scottish National Memorial to David Livingstone Trust.</t>
+  </si>
+  <si>
+    <t>liv_016263</t>
+  </si>
+  <si>
+    <t>liv_016264</t>
+  </si>
+  <si>
+    <t>liv_016265</t>
+  </si>
+  <si>
+    <t>liv_016266</t>
+  </si>
+  <si>
+    <t>liv_016267</t>
+  </si>
+  <si>
+    <t>liv_016268</t>
+  </si>
+  <si>
+    <t>liv_016269</t>
+  </si>
+  <si>
+    <t>Auction advertisement for David Livingstone, Letter to Richard Owen, 26 December 1864, [1970s?]</t>
+  </si>
+  <si>
+    <t>Auction advertisement for David Livingstone, Letter to Richard Owen, 26 December 1864</t>
+  </si>
+  <si>
+    <t>1970s</t>
+  </si>
+  <si>
+    <t>1970/1979</t>
+  </si>
+  <si>
+    <t>Elmer L. Andersen Library, University of Minnesota</t>
+  </si>
+  <si>
+    <t>Elmer L. Andersen Library, University of Minnesota, 2018</t>
+  </si>
+  <si>
+    <t>Archival box that holds Livingstone manuscript, Elmer L. Andersen Library, University of Minnesota</t>
+  </si>
+  <si>
+    <t>Archival box that holds Livingstone manuscript, Elmer L. Andersen Library, University of Minnesota, 2018</t>
   </si>
 </sst>
 </file>
@@ -10131,7 +10176,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="916">
+  <cellStyleXfs count="928">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -10193,6 +10238,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11262,7 +11319,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="916">
+  <cellStyles count="928">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -11729,6 +11786,12 @@
     <cellStyle name="Followed Hyperlink" xfId="911" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="913" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="915" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="917" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="919" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="921" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="923" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="925" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="927" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -12178,6 +12241,12 @@
     <cellStyle name="Hyperlink" xfId="910" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="912" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="914" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="916" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="918" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="920" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="922" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="924" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="926" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -12507,11 +12576,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1202"/>
+  <dimension ref="A1:P1209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1202" sqref="P1202"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1203" sqref="A1203:XFD1209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -61415,6 +61484,251 @@
         <v>3321</v>
       </c>
     </row>
+    <row r="1203" spans="1:16" ht="45">
+      <c r="A1203" s="28" t="s">
+        <v>3322</v>
+      </c>
+      <c r="B1203" s="17" t="s">
+        <v>3333</v>
+      </c>
+      <c r="C1203" s="17" t="s">
+        <v>3334</v>
+      </c>
+      <c r="F1203" s="9" t="s">
+        <v>2436</v>
+      </c>
+      <c r="G1203" s="69" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1203" s="69" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1203" s="69" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1203" s="12">
+        <v>2018</v>
+      </c>
+      <c r="K1203" s="12">
+        <v>2018</v>
+      </c>
+      <c r="L1203" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P1203" s="69" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:16" ht="45">
+      <c r="A1204" s="28" t="s">
+        <v>3323</v>
+      </c>
+      <c r="B1204" s="17" t="s">
+        <v>3333</v>
+      </c>
+      <c r="C1204" s="17" t="s">
+        <v>3334</v>
+      </c>
+      <c r="F1204" s="9" t="s">
+        <v>2436</v>
+      </c>
+      <c r="G1204" s="69" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1204" s="69" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1204" s="69" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1204" s="12">
+        <v>2018</v>
+      </c>
+      <c r="K1204" s="12">
+        <v>2018</v>
+      </c>
+      <c r="L1204" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P1204" s="69" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:16" ht="45">
+      <c r="A1205" s="28" t="s">
+        <v>3324</v>
+      </c>
+      <c r="B1205" s="17" t="s">
+        <v>3333</v>
+      </c>
+      <c r="C1205" s="17" t="s">
+        <v>3334</v>
+      </c>
+      <c r="F1205" s="9" t="s">
+        <v>2436</v>
+      </c>
+      <c r="G1205" s="69" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1205" s="69" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1205" s="69" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1205" s="12">
+        <v>2018</v>
+      </c>
+      <c r="K1205" s="12">
+        <v>2018</v>
+      </c>
+      <c r="L1205" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P1205" s="69" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:16" ht="45">
+      <c r="A1206" s="28" t="s">
+        <v>3325</v>
+      </c>
+      <c r="B1206" s="17" t="s">
+        <v>3333</v>
+      </c>
+      <c r="C1206" s="17" t="s">
+        <v>3334</v>
+      </c>
+      <c r="F1206" s="9" t="s">
+        <v>2436</v>
+      </c>
+      <c r="G1206" s="69" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1206" s="69" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1206" s="69" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1206" s="12">
+        <v>2018</v>
+      </c>
+      <c r="K1206" s="12">
+        <v>2018</v>
+      </c>
+      <c r="L1206" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P1206" s="69" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:16" ht="45">
+      <c r="A1207" s="28" t="s">
+        <v>3326</v>
+      </c>
+      <c r="B1207" s="17" t="s">
+        <v>3333</v>
+      </c>
+      <c r="C1207" s="17" t="s">
+        <v>3334</v>
+      </c>
+      <c r="F1207" s="9" t="s">
+        <v>2436</v>
+      </c>
+      <c r="G1207" s="69" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1207" s="69" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1207" s="69" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1207" s="12">
+        <v>2018</v>
+      </c>
+      <c r="K1207" s="12">
+        <v>2018</v>
+      </c>
+      <c r="L1207" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P1207" s="69" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:16" ht="45">
+      <c r="A1208" s="28" t="s">
+        <v>3327</v>
+      </c>
+      <c r="B1208" s="17" t="s">
+        <v>3335</v>
+      </c>
+      <c r="C1208" s="17" t="s">
+        <v>3336</v>
+      </c>
+      <c r="F1208" s="9" t="s">
+        <v>2436</v>
+      </c>
+      <c r="G1208" s="69" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1208" s="69" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1208" s="69" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1208" s="12">
+        <v>2018</v>
+      </c>
+      <c r="K1208" s="12">
+        <v>2018</v>
+      </c>
+      <c r="L1208" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P1208" s="69" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:16" ht="45">
+      <c r="A1209" s="28" t="s">
+        <v>3328</v>
+      </c>
+      <c r="B1209" s="17" t="s">
+        <v>3330</v>
+      </c>
+      <c r="C1209" s="17" t="s">
+        <v>3329</v>
+      </c>
+      <c r="F1209" s="9" t="s">
+        <v>2436</v>
+      </c>
+      <c r="G1209" s="69" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H1209" s="69" t="s">
+        <v>1144</v>
+      </c>
+      <c r="I1209" s="69" t="s">
+        <v>972</v>
+      </c>
+      <c r="J1209" s="12" t="s">
+        <v>3331</v>
+      </c>
+      <c r="K1209" s="12" t="s">
+        <v>3332</v>
+      </c>
+      <c r="L1209" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P1209" s="69" t="s">
+        <v>2588</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>